<commit_message>
L.K | 12/09/2023 16:55 | Criadas as funções de extração da capa de dados, de extração das partes representantes, de processos relacionados. A função de screenshot está 30% concluída.
</commit_message>
<xml_diff>
--- a/testes/teste_pre_dot.xlsx
+++ b/testes/teste_pre_dot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Área de Trabalho\a01_codigos\a16_LegalTrackHub\testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDAF1D8-B8C7-491F-801F-BA7F58CD7C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5D4AC6-E50C-46A2-8B2D-5068BA55252A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -401,12 +401,12 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E10:E11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -416,57 +416,57 @@
     </row>
     <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>